<commit_message>
Finished Shafts Analysis File
</commit_message>
<xml_diff>
--- a/Athletis Shaft Analysis File/Lot Report.xlsx
+++ b/Athletis Shaft Analysis File/Lot Report.xlsx
@@ -2,24 +2,24 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Quinnzy\Documents\DataAnalysisTrials\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450"/>
   </bookViews>
   <sheets>
-    <sheet name="03" sheetId="1" r:id="rId1"/>
+    <sheet name="04" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="35">
   <si>
     <t>SID</t>
   </si>
@@ -111,13 +111,13 @@
     <t>Smiley_Mandrel_Check</t>
   </si>
   <si>
-    <t>91164963-03</t>
+    <t>91164963-04</t>
   </si>
   <si>
     <t>AK Line 19</t>
   </si>
   <si>
-    <t>Christopher O'Connor</t>
+    <t>Brendan Treacy</t>
   </si>
   <si>
     <t>Collection</t>
@@ -130,9 +130,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0000000000"/>
-  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -195,7 +192,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C5700"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -588,32 +585,32 @@
     <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -689,7 +686,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -701,7 +698,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -748,23 +745,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -800,23 +780,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -969,15 +932,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG11"/>
+  <dimension ref="A1:AG41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="G3" sqref="G3:G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.25">
@@ -1083,7 +1046,7 @@
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1586259941</v>
+        <v>1586284765</v>
       </c>
       <c r="B2" t="s">
         <v>30</v>
@@ -1092,7 +1055,7 @@
         <v>31</v>
       </c>
       <c r="D2">
-        <v>25442539</v>
+        <v>25443020</v>
       </c>
       <c r="E2" t="s">
         <v>32</v>
@@ -1101,7 +1064,7 @@
         <v>43928</v>
       </c>
       <c r="G2" s="2">
-        <v>0.28171296296296294</v>
+        <v>0.56901620370370376</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -1113,49 +1076,49 @@
         <v>33</v>
       </c>
       <c r="K2">
+        <v>0.16159999999999999</v>
+      </c>
+      <c r="L2">
+        <v>0.16400000000000001</v>
+      </c>
+      <c r="M2">
+        <v>0.51</v>
+      </c>
+      <c r="N2">
+        <v>0.12</v>
+      </c>
+      <c r="O2">
+        <v>1570</v>
+      </c>
+      <c r="P2">
+        <v>6.0400000000000002E-2</v>
+      </c>
+      <c r="Q2">
+        <v>1.9253</v>
+      </c>
+      <c r="R2">
+        <v>-1.6000000000000001E-3</v>
+      </c>
+      <c r="S2">
+        <v>0.16</v>
+      </c>
+      <c r="T2">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="U2">
         <v>0.16439999999999999</v>
       </c>
-      <c r="L2">
-        <v>0.16880000000000001</v>
-      </c>
-      <c r="M2">
-        <v>0.50800000000000001</v>
-      </c>
-      <c r="N2">
-        <v>0.1148</v>
-      </c>
-      <c r="O2">
-        <v>950</v>
-      </c>
-      <c r="P2">
-        <v>6.5000000000000002E-2</v>
-      </c>
-      <c r="Q2">
-        <v>1.8998999999999999</v>
-      </c>
-      <c r="R2">
-        <v>-4.0000000000000002E-4</v>
-      </c>
-      <c r="S2">
-        <v>0.16400000000000001</v>
-      </c>
-      <c r="T2">
-        <v>-8.0000000000000004E-4</v>
-      </c>
-      <c r="U2">
-        <v>0.16800000000000001</v>
-      </c>
       <c r="V2">
-        <v>1.6000000000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="W2">
-        <v>0.50960000000000005</v>
+        <v>0.51</v>
       </c>
       <c r="X2">
         <v>0</v>
       </c>
       <c r="Y2">
-        <v>0.1148</v>
+        <v>0.12</v>
       </c>
       <c r="Z2">
         <v>0</v>
@@ -1184,7 +1147,7 @@
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1586259849</v>
+        <v>1586284723</v>
       </c>
       <c r="B3" t="s">
         <v>30</v>
@@ -1193,7 +1156,7 @@
         <v>31</v>
       </c>
       <c r="D3">
-        <v>25442539</v>
+        <v>25443020</v>
       </c>
       <c r="E3" t="s">
         <v>32</v>
@@ -1202,7 +1165,7 @@
         <v>43928</v>
       </c>
       <c r="G3" s="2">
-        <v>0.28065972222222224</v>
+        <v>0.56854166666666661</v>
       </c>
       <c r="H3">
         <v>1</v>
@@ -1214,43 +1177,43 @@
         <v>33</v>
       </c>
       <c r="K3">
-        <v>0.17560000000000001</v>
+        <v>0.16120000000000001</v>
       </c>
       <c r="L3">
-        <v>0.16639999999999999</v>
+        <v>0.16839999999999999</v>
       </c>
       <c r="M3">
-        <v>0.50319999999999998</v>
+        <v>0.50600000000000001</v>
       </c>
       <c r="N3">
         <v>0.1188</v>
       </c>
       <c r="O3">
-        <v>950</v>
+        <v>1570</v>
       </c>
       <c r="P3">
-        <v>8.2900000000000001E-2</v>
+        <v>5.7099999999999998E-2</v>
       </c>
       <c r="Q3">
-        <v>1.903</v>
+        <v>1.9224000000000001</v>
       </c>
       <c r="R3">
-        <v>-1.6000000000000001E-3</v>
+        <v>-4.0000000000000002E-4</v>
       </c>
       <c r="S3">
-        <v>0.17399999999999999</v>
+        <v>0.1608</v>
       </c>
       <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <v>0.16839999999999999</v>
+      </c>
+      <c r="V3">
         <v>-4.0000000000000002E-4</v>
       </c>
-      <c r="U3">
-        <v>0.16600000000000001</v>
-      </c>
-      <c r="V3">
-        <v>0.1736</v>
-      </c>
       <c r="W3">
-        <v>0.67679999999999996</v>
+        <v>0.50560000000000005</v>
       </c>
       <c r="X3">
         <v>0</v>
@@ -1285,7 +1248,7 @@
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1586259378</v>
+        <v>1586284067</v>
       </c>
       <c r="B4" t="s">
         <v>30</v>
@@ -1294,7 +1257,7 @@
         <v>31</v>
       </c>
       <c r="D4">
-        <v>25442539</v>
+        <v>25443020</v>
       </c>
       <c r="E4" t="s">
         <v>32</v>
@@ -1303,7 +1266,7 @@
         <v>43928</v>
       </c>
       <c r="G4" s="2">
-        <v>0.27520833333333333</v>
+        <v>0.56093749999999998</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -1315,43 +1278,43 @@
         <v>33</v>
       </c>
       <c r="K4">
-        <v>0.1696</v>
+        <v>0.1608</v>
       </c>
       <c r="L4">
-        <v>0.1668</v>
+        <v>0.16320000000000001</v>
       </c>
       <c r="M4">
-        <v>0.50160000000000005</v>
+        <v>0.50600000000000001</v>
       </c>
       <c r="N4">
         <v>0.1192</v>
       </c>
       <c r="O4">
-        <v>950</v>
+        <v>1570</v>
       </c>
       <c r="P4">
-        <v>8.0100000000000005E-2</v>
+        <v>6.1899999999999997E-2</v>
       </c>
       <c r="Q4">
-        <v>1.8918999999999999</v>
+        <v>1.9173</v>
       </c>
       <c r="R4">
-        <v>-1.1999999999999999E-3</v>
+        <v>0</v>
       </c>
       <c r="S4">
-        <v>0.16839999999999999</v>
+        <v>0.1608</v>
       </c>
       <c r="T4">
-        <v>1.1135999999999999</v>
+        <v>-4.0000000000000002E-4</v>
       </c>
       <c r="U4">
-        <v>1.2804</v>
+        <v>0.1628</v>
       </c>
       <c r="V4">
-        <v>0.16839999999999999</v>
+        <v>0</v>
       </c>
       <c r="W4">
-        <v>0.67</v>
+        <v>0.50600000000000001</v>
       </c>
       <c r="X4">
         <v>0</v>
@@ -1386,7 +1349,7 @@
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>1586259310</v>
+        <v>1586283999</v>
       </c>
       <c r="B5" t="s">
         <v>30</v>
@@ -1395,7 +1358,7 @@
         <v>31</v>
       </c>
       <c r="D5">
-        <v>25442539</v>
+        <v>25443020</v>
       </c>
       <c r="E5" t="s">
         <v>32</v>
@@ -1404,7 +1367,7 @@
         <v>43928</v>
       </c>
       <c r="G5" s="2">
-        <v>0.27439814814814817</v>
+        <v>0.56016203703703704</v>
       </c>
       <c r="H5">
         <v>1</v>
@@ -1416,49 +1379,49 @@
         <v>33</v>
       </c>
       <c r="K5">
-        <v>0.1676</v>
+        <v>0.16239999999999999</v>
       </c>
       <c r="L5">
-        <v>0.15840000000000001</v>
+        <v>0.16400000000000001</v>
       </c>
       <c r="M5">
-        <v>0.50839999999999996</v>
+        <v>0.50960000000000005</v>
       </c>
       <c r="N5">
-        <v>0.1172</v>
+        <v>0.1216</v>
       </c>
       <c r="O5">
-        <v>950</v>
+        <v>1570</v>
       </c>
       <c r="P5">
-        <v>7.3400000000000007E-2</v>
+        <v>6.0499999999999998E-2</v>
       </c>
       <c r="Q5">
-        <v>1.9036999999999999</v>
+        <v>1.9092</v>
       </c>
       <c r="R5">
-        <v>-1.1999999999999999E-3</v>
+        <v>-4.0000000000000002E-4</v>
       </c>
       <c r="S5">
-        <v>0.16639999999999999</v>
+        <v>0.16200000000000001</v>
       </c>
       <c r="T5">
-        <v>1.79</v>
+        <v>0</v>
       </c>
       <c r="U5">
-        <v>1.9483999999999999</v>
+        <v>0.16400000000000001</v>
       </c>
       <c r="V5">
-        <v>0.16639999999999999</v>
+        <v>0</v>
       </c>
       <c r="W5">
-        <v>0.67479999999999996</v>
+        <v>0.50960000000000005</v>
       </c>
       <c r="X5">
-        <v>0</v>
+        <v>-4.0000000000000002E-4</v>
       </c>
       <c r="Y5">
-        <v>0.1172</v>
+        <v>0.1212</v>
       </c>
       <c r="Z5">
         <v>0</v>
@@ -1487,7 +1450,7 @@
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>1586257886</v>
+        <v>1586283691</v>
       </c>
       <c r="B6" t="s">
         <v>30</v>
@@ -1496,7 +1459,7 @@
         <v>31</v>
       </c>
       <c r="D6">
-        <v>25442539</v>
+        <v>25443020</v>
       </c>
       <c r="E6" t="s">
         <v>32</v>
@@ -1505,7 +1468,7 @@
         <v>43928</v>
       </c>
       <c r="G6" s="2">
-        <v>0.25793981481481482</v>
+        <v>0.55660879629629634</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -1517,49 +1480,49 @@
         <v>33</v>
       </c>
       <c r="K6">
-        <v>0.1628</v>
+        <v>0.16439999999999999</v>
       </c>
       <c r="L6">
-        <v>0.16120000000000001</v>
+        <v>0.16400000000000001</v>
       </c>
       <c r="M6">
-        <v>0.50160000000000005</v>
+        <v>0.50760000000000005</v>
       </c>
       <c r="N6">
-        <v>0.1144</v>
+        <v>0.122</v>
       </c>
       <c r="O6">
-        <v>950</v>
+        <v>1570</v>
       </c>
       <c r="P6">
-        <v>7.9299999999999995E-2</v>
+        <v>5.6599999999999998E-2</v>
       </c>
       <c r="Q6">
-        <v>1.9046000000000001</v>
+        <v>1.9156</v>
       </c>
       <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>0.16439999999999999</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <v>0.16400000000000001</v>
+      </c>
+      <c r="V6">
         <v>-4.0000000000000002E-4</v>
       </c>
-      <c r="S6">
-        <v>0.16239999999999999</v>
-      </c>
-      <c r="T6">
-        <v>1.7676000000000001</v>
-      </c>
-      <c r="U6">
-        <v>1.9288000000000001</v>
-      </c>
-      <c r="V6">
-        <v>0.16239999999999999</v>
-      </c>
       <c r="W6">
-        <v>0.66400000000000003</v>
+        <v>0.50719999999999998</v>
       </c>
       <c r="X6">
-        <v>0.66479999999999995</v>
+        <v>0</v>
       </c>
       <c r="Y6">
-        <v>0.7792</v>
+        <v>0.122</v>
       </c>
       <c r="Z6">
         <v>0</v>
@@ -1588,7 +1551,7 @@
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>1586257832</v>
+        <v>1586283649</v>
       </c>
       <c r="B7" t="s">
         <v>30</v>
@@ -1597,7 +1560,7 @@
         <v>31</v>
       </c>
       <c r="D7">
-        <v>25442539</v>
+        <v>25443020</v>
       </c>
       <c r="E7" t="s">
         <v>32</v>
@@ -1606,7 +1569,7 @@
         <v>43928</v>
       </c>
       <c r="G7" s="2">
-        <v>0.25731481481481483</v>
+        <v>0.55608796296296303</v>
       </c>
       <c r="H7">
         <v>1</v>
@@ -1618,49 +1581,49 @@
         <v>33</v>
       </c>
       <c r="K7">
-        <v>0.1608</v>
+        <v>0.15920000000000001</v>
       </c>
       <c r="L7">
-        <v>0.1636</v>
+        <v>0.16919999999999999</v>
       </c>
       <c r="M7">
-        <v>0.49719999999999998</v>
+        <v>0.49919999999999998</v>
       </c>
       <c r="N7">
-        <v>0.1192</v>
+        <v>0.122</v>
       </c>
       <c r="O7">
-        <v>950</v>
+        <v>1570</v>
       </c>
       <c r="P7">
-        <v>6.9900000000000004E-2</v>
+        <v>5.4899999999999997E-2</v>
       </c>
       <c r="Q7">
-        <v>1.9037999999999999</v>
+        <v>1.9129</v>
       </c>
       <c r="R7">
         <v>-4.0000000000000002E-4</v>
       </c>
       <c r="S7">
-        <v>0.16039999999999999</v>
+        <v>0.1588</v>
       </c>
       <c r="T7">
-        <v>1.5992</v>
+        <v>-1.1999999999999999E-3</v>
       </c>
       <c r="U7">
-        <v>1.7627999999999999</v>
+        <v>0.16800000000000001</v>
       </c>
       <c r="V7">
         <v>0</v>
       </c>
       <c r="W7">
-        <v>0.49719999999999998</v>
+        <v>0.49919999999999998</v>
       </c>
       <c r="X7">
-        <v>0.49719999999999998</v>
+        <v>0</v>
       </c>
       <c r="Y7">
-        <v>0.61639999999999995</v>
+        <v>0.122</v>
       </c>
       <c r="Z7">
         <v>0</v>
@@ -1689,7 +1652,7 @@
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>1586257582</v>
+        <v>1586282963</v>
       </c>
       <c r="B8" t="s">
         <v>30</v>
@@ -1698,7 +1661,7 @@
         <v>31</v>
       </c>
       <c r="D8">
-        <v>25442539</v>
+        <v>25443020</v>
       </c>
       <c r="E8" t="s">
         <v>32</v>
@@ -1707,7 +1670,7 @@
         <v>43928</v>
       </c>
       <c r="G8" s="2">
-        <v>0.25442129629629628</v>
+        <v>0.54818287037037039</v>
       </c>
       <c r="H8">
         <v>1</v>
@@ -1719,49 +1682,49 @@
         <v>33</v>
       </c>
       <c r="K8">
+        <v>0.16120000000000001</v>
+      </c>
+      <c r="L8">
         <v>0.16320000000000001</v>
       </c>
-      <c r="L8">
-        <v>0.15959999999999999</v>
-      </c>
       <c r="M8">
-        <v>0.4884</v>
+        <v>0.50360000000000005</v>
       </c>
       <c r="N8">
         <v>0.1196</v>
       </c>
       <c r="O8">
-        <v>950</v>
+        <v>1570</v>
       </c>
       <c r="P8">
-        <v>7.6799999999999993E-2</v>
+        <v>6.0100000000000001E-2</v>
       </c>
       <c r="Q8">
-        <v>1.9056999999999999</v>
+        <v>1.9185000000000001</v>
       </c>
       <c r="R8">
-        <v>-8.0000000000000004E-4</v>
+        <v>-4.0000000000000002E-4</v>
       </c>
       <c r="S8">
-        <v>0.16239999999999999</v>
+        <v>0.1608</v>
       </c>
       <c r="T8">
-        <v>-8.0000000000000004E-4</v>
+        <v>-4.0000000000000002E-4</v>
       </c>
       <c r="U8">
-        <v>0.1588</v>
+        <v>0.1628</v>
       </c>
       <c r="V8">
-        <v>-1.1999999999999999E-3</v>
+        <v>0</v>
       </c>
       <c r="W8">
-        <v>0.48720000000000002</v>
+        <v>0.50360000000000005</v>
       </c>
       <c r="X8">
-        <v>-4.0000000000000002E-4</v>
+        <v>0</v>
       </c>
       <c r="Y8">
-        <v>0.1192</v>
+        <v>0.1196</v>
       </c>
       <c r="Z8">
         <v>0</v>
@@ -1790,7 +1753,7 @@
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>1586257253</v>
+        <v>1586282916</v>
       </c>
       <c r="B9" t="s">
         <v>30</v>
@@ -1799,7 +1762,7 @@
         <v>31</v>
       </c>
       <c r="D9">
-        <v>25442539</v>
+        <v>25443020</v>
       </c>
       <c r="E9" t="s">
         <v>32</v>
@@ -1808,7 +1771,7 @@
         <v>43928</v>
       </c>
       <c r="G9" s="2">
-        <v>0.25061342592592589</v>
+        <v>0.54762731481481486</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -1820,49 +1783,49 @@
         <v>33</v>
       </c>
       <c r="K9">
-        <v>0.17080000000000001</v>
+        <v>0.17</v>
       </c>
       <c r="L9">
-        <v>0.16880000000000001</v>
+        <v>0.16159999999999999</v>
       </c>
       <c r="M9">
-        <v>0.48959999999999998</v>
+        <v>0.50600000000000001</v>
       </c>
       <c r="N9">
+        <v>0.1212</v>
+      </c>
+      <c r="O9">
+        <v>1570</v>
+      </c>
+      <c r="P9">
+        <v>5.8299999999999998E-2</v>
+      </c>
+      <c r="Q9">
+        <v>1.925</v>
+      </c>
+      <c r="R9">
+        <v>-8.0000000000000004E-4</v>
+      </c>
+      <c r="S9">
+        <v>0.16919999999999999</v>
+      </c>
+      <c r="T9">
+        <v>0</v>
+      </c>
+      <c r="U9">
+        <v>0.16159999999999999</v>
+      </c>
+      <c r="V9">
+        <v>0</v>
+      </c>
+      <c r="W9">
+        <v>0.50600000000000001</v>
+      </c>
+      <c r="X9">
+        <v>-4.0000000000000002E-4</v>
+      </c>
+      <c r="Y9">
         <v>0.1208</v>
-      </c>
-      <c r="O9">
-        <v>950</v>
-      </c>
-      <c r="P9">
-        <v>7.6700000000000004E-2</v>
-      </c>
-      <c r="Q9">
-        <v>1.8980999999999999</v>
-      </c>
-      <c r="R9">
-        <v>0</v>
-      </c>
-      <c r="S9">
-        <v>0.17080000000000001</v>
-      </c>
-      <c r="T9">
-        <v>-4.0000000000000002E-4</v>
-      </c>
-      <c r="U9">
-        <v>0.16839999999999999</v>
-      </c>
-      <c r="V9">
-        <v>0</v>
-      </c>
-      <c r="W9">
-        <v>0.48959999999999998</v>
-      </c>
-      <c r="X9">
-        <v>0.48720000000000002</v>
-      </c>
-      <c r="Y9">
-        <v>0.60799999999999998</v>
       </c>
       <c r="Z9">
         <v>0</v>
@@ -1891,7 +1854,7 @@
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>1586255444</v>
+        <v>1586282233</v>
       </c>
       <c r="B10" t="s">
         <v>30</v>
@@ -1900,7 +1863,7 @@
         <v>31</v>
       </c>
       <c r="D10">
-        <v>25442539</v>
+        <v>25443020</v>
       </c>
       <c r="E10" t="s">
         <v>32</v>
@@ -1909,7 +1872,7 @@
         <v>43928</v>
       </c>
       <c r="G10" s="2">
-        <v>0.22964120370370369</v>
+        <v>0.53973379629629636</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -1921,49 +1884,49 @@
         <v>33</v>
       </c>
       <c r="K10">
-        <v>0.16120000000000001</v>
+        <v>0.16200000000000001</v>
       </c>
       <c r="L10">
-        <v>0.1636</v>
+        <v>0.16239999999999999</v>
       </c>
       <c r="M10">
-        <v>0.49480000000000002</v>
+        <v>0.50360000000000005</v>
       </c>
       <c r="N10">
-        <v>0.12280000000000001</v>
+        <v>0.1188</v>
       </c>
       <c r="O10">
-        <v>950</v>
+        <v>1570</v>
       </c>
       <c r="P10">
-        <v>5.7599999999999998E-2</v>
+        <v>5.9900000000000002E-2</v>
       </c>
       <c r="Q10">
-        <v>1.9069</v>
+        <v>1.9269000000000001</v>
       </c>
       <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="T10">
         <v>-4.0000000000000002E-4</v>
       </c>
-      <c r="S10">
-        <v>0.1608</v>
-      </c>
-      <c r="T10">
-        <v>1.774</v>
-      </c>
       <c r="U10">
-        <v>1.9376</v>
+        <v>0.16200000000000001</v>
       </c>
       <c r="V10">
-        <v>0.16200000000000001</v>
+        <v>0</v>
       </c>
       <c r="W10">
-        <v>0.65680000000000005</v>
+        <v>0.50360000000000005</v>
       </c>
       <c r="X10">
-        <v>0.65839999999999999</v>
+        <v>-4.0000000000000002E-4</v>
       </c>
       <c r="Y10">
-        <v>0.78120000000000001</v>
+        <v>0.11840000000000001</v>
       </c>
       <c r="Z10">
         <v>0</v>
@@ -1992,7 +1955,7 @@
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>1586255386</v>
+        <v>1586282159</v>
       </c>
       <c r="B11" t="s">
         <v>30</v>
@@ -2001,7 +1964,7 @@
         <v>31</v>
       </c>
       <c r="D11">
-        <v>25442539</v>
+        <v>25443020</v>
       </c>
       <c r="E11" t="s">
         <v>32</v>
@@ -2010,7 +1973,7 @@
         <v>43928</v>
       </c>
       <c r="G11" s="2">
-        <v>0.22900462962962964</v>
+        <v>0.53887731481481482</v>
       </c>
       <c r="H11">
         <v>1</v>
@@ -2022,77 +1985,3106 @@
         <v>33</v>
       </c>
       <c r="K11">
-        <v>0.16520000000000001</v>
+        <v>0.15959999999999999</v>
       </c>
       <c r="L11">
         <v>0.16520000000000001</v>
       </c>
       <c r="M11">
-        <v>0.49559999999999998</v>
+        <v>0.50839999999999996</v>
       </c>
       <c r="N11">
-        <v>0.122</v>
+        <v>0.1168</v>
       </c>
       <c r="O11">
-        <v>950</v>
+        <v>1570</v>
       </c>
       <c r="P11">
-        <v>7.1300000000000002E-2</v>
+        <v>6.1499999999999999E-2</v>
       </c>
       <c r="Q11">
-        <v>1.9086000000000001</v>
+        <v>1.9253</v>
       </c>
       <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>0.15959999999999999</v>
+      </c>
+      <c r="T11">
+        <v>-4.0000000000000002E-4</v>
+      </c>
+      <c r="U11">
+        <v>0.1648</v>
+      </c>
+      <c r="V11">
+        <v>0</v>
+      </c>
+      <c r="W11">
+        <v>0.50839999999999996</v>
+      </c>
+      <c r="X11">
+        <v>0</v>
+      </c>
+      <c r="Y11">
+        <v>0.1168</v>
+      </c>
+      <c r="Z11">
+        <v>0</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB11">
+        <v>0</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD11">
+        <v>0</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF11">
+        <v>0</v>
+      </c>
+      <c r="AG11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1586281650</v>
+      </c>
+      <c r="B12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12">
+        <v>25443020</v>
+      </c>
+      <c r="E12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="1">
+        <v>43928</v>
+      </c>
+      <c r="G12" s="2">
+        <v>0.53298611111111105</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12" t="s">
+        <v>33</v>
+      </c>
+      <c r="K12">
+        <v>0.1608</v>
+      </c>
+      <c r="L12">
+        <v>0.16400000000000001</v>
+      </c>
+      <c r="M12">
+        <v>0.50319999999999998</v>
+      </c>
+      <c r="N12">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="O12">
+        <v>1570</v>
+      </c>
+      <c r="P12">
+        <v>5.9400000000000001E-2</v>
+      </c>
+      <c r="Q12">
+        <v>1.9179999999999999</v>
+      </c>
+      <c r="R12">
+        <v>0</v>
+      </c>
+      <c r="S12">
+        <v>0.1608</v>
+      </c>
+      <c r="T12">
+        <v>-4.0000000000000002E-4</v>
+      </c>
+      <c r="U12">
+        <v>0.1636</v>
+      </c>
+      <c r="V12">
+        <v>-4.0000000000000002E-4</v>
+      </c>
+      <c r="W12">
+        <v>0.50280000000000002</v>
+      </c>
+      <c r="X12">
+        <v>-4.0000000000000002E-4</v>
+      </c>
+      <c r="Y12">
+        <v>0.1176</v>
+      </c>
+      <c r="Z12">
+        <v>0</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB12">
+        <v>0</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD12">
+        <v>0</v>
+      </c>
+      <c r="AE12" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF12">
+        <v>0</v>
+      </c>
+      <c r="AG12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1586281602</v>
+      </c>
+      <c r="B13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13">
+        <v>25443020</v>
+      </c>
+      <c r="E13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="1">
+        <v>43928</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0.53243055555555563</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="J13" t="s">
+        <v>33</v>
+      </c>
+      <c r="K13">
+        <v>0.158</v>
+      </c>
+      <c r="L13">
+        <v>0.16439999999999999</v>
+      </c>
+      <c r="M13">
+        <v>0.50760000000000005</v>
+      </c>
+      <c r="N13">
+        <v>0.1212</v>
+      </c>
+      <c r="O13">
+        <v>1570</v>
+      </c>
+      <c r="P13">
+        <v>5.57E-2</v>
+      </c>
+      <c r="Q13">
+        <v>1.9197</v>
+      </c>
+      <c r="R13">
+        <v>-4.0000000000000002E-4</v>
+      </c>
+      <c r="S13">
+        <v>0.15759999999999999</v>
+      </c>
+      <c r="T13">
+        <v>-4.0000000000000002E-4</v>
+      </c>
+      <c r="U13">
+        <v>0.16400000000000001</v>
+      </c>
+      <c r="V13">
+        <v>0</v>
+      </c>
+      <c r="W13">
+        <v>0.50760000000000005</v>
+      </c>
+      <c r="X13">
+        <v>0</v>
+      </c>
+      <c r="Y13">
+        <v>0.1212</v>
+      </c>
+      <c r="Z13">
+        <v>0</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB13">
+        <v>0</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD13">
+        <v>0</v>
+      </c>
+      <c r="AE13" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF13">
+        <v>0</v>
+      </c>
+      <c r="AG13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1586280888</v>
+      </c>
+      <c r="B14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14">
+        <v>25443020</v>
+      </c>
+      <c r="E14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="1">
+        <v>43928</v>
+      </c>
+      <c r="G14" s="2">
+        <v>0.52416666666666667</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="J14" t="s">
+        <v>33</v>
+      </c>
+      <c r="K14">
+        <v>0.15959999999999999</v>
+      </c>
+      <c r="L14">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="M14">
+        <v>0.50560000000000005</v>
+      </c>
+      <c r="N14">
+        <v>0.1208</v>
+      </c>
+      <c r="O14">
+        <v>1570</v>
+      </c>
+      <c r="P14">
+        <v>5.9700000000000003E-2</v>
+      </c>
+      <c r="Q14">
+        <v>1.9205000000000001</v>
+      </c>
+      <c r="R14">
+        <v>-4.0000000000000002E-4</v>
+      </c>
+      <c r="S14">
+        <v>0.15920000000000001</v>
+      </c>
+      <c r="T14">
+        <v>0</v>
+      </c>
+      <c r="U14">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="V14">
+        <v>0</v>
+      </c>
+      <c r="W14">
+        <v>0.50560000000000005</v>
+      </c>
+      <c r="X14">
+        <v>0</v>
+      </c>
+      <c r="Y14">
+        <v>0.1208</v>
+      </c>
+      <c r="Z14">
+        <v>0</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB14">
+        <v>0</v>
+      </c>
+      <c r="AC14" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD14">
+        <v>0</v>
+      </c>
+      <c r="AE14" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF14">
+        <v>0</v>
+      </c>
+      <c r="AG14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1586280841</v>
+      </c>
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15">
+        <v>25443020</v>
+      </c>
+      <c r="E15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="1">
+        <v>43928</v>
+      </c>
+      <c r="G15" s="2">
+        <v>0.52362268518518518</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15" t="s">
+        <v>33</v>
+      </c>
+      <c r="K15">
+        <v>0.16</v>
+      </c>
+      <c r="L15">
+        <v>0.1648</v>
+      </c>
+      <c r="M15">
+        <v>0.51039999999999996</v>
+      </c>
+      <c r="N15">
+        <v>0.1188</v>
+      </c>
+      <c r="O15">
+        <v>1570</v>
+      </c>
+      <c r="P15">
+        <v>5.9499999999999997E-2</v>
+      </c>
+      <c r="Q15">
+        <v>1.9239999999999999</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <v>0.16</v>
+      </c>
+      <c r="T15">
+        <v>0</v>
+      </c>
+      <c r="U15">
+        <v>0.1648</v>
+      </c>
+      <c r="V15">
+        <v>0</v>
+      </c>
+      <c r="W15">
+        <v>0.51039999999999996</v>
+      </c>
+      <c r="X15">
+        <v>0</v>
+      </c>
+      <c r="Y15">
+        <v>0.1188</v>
+      </c>
+      <c r="Z15">
+        <v>0</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB15">
+        <v>0</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD15">
+        <v>0</v>
+      </c>
+      <c r="AE15" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF15">
+        <v>0</v>
+      </c>
+      <c r="AG15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1586280462</v>
+      </c>
+      <c r="B16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16">
+        <v>25443020</v>
+      </c>
+      <c r="E16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16" s="1">
+        <v>43928</v>
+      </c>
+      <c r="G16" s="2">
+        <v>0.51923611111111112</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="J16" t="s">
+        <v>33</v>
+      </c>
+      <c r="K16">
+        <v>0.16159999999999999</v>
+      </c>
+      <c r="L16">
+        <v>0.16439999999999999</v>
+      </c>
+      <c r="M16">
+        <v>0.50680000000000003</v>
+      </c>
+      <c r="N16">
+        <v>0.1188</v>
+      </c>
+      <c r="O16">
+        <v>1570</v>
+      </c>
+      <c r="P16">
+        <v>6.2799999999999995E-2</v>
+      </c>
+      <c r="Q16">
+        <v>1.9258999999999999</v>
+      </c>
+      <c r="R16">
+        <v>0</v>
+      </c>
+      <c r="S16">
+        <v>0.16159999999999999</v>
+      </c>
+      <c r="T16">
+        <v>0</v>
+      </c>
+      <c r="U16">
+        <v>0.16439999999999999</v>
+      </c>
+      <c r="V16">
+        <v>0</v>
+      </c>
+      <c r="W16">
+        <v>0.50680000000000003</v>
+      </c>
+      <c r="X16">
+        <v>-4.0000000000000002E-4</v>
+      </c>
+      <c r="Y16">
+        <v>0.11840000000000001</v>
+      </c>
+      <c r="Z16">
+        <v>0</v>
+      </c>
+      <c r="AA16" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB16">
+        <v>0</v>
+      </c>
+      <c r="AC16" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD16">
+        <v>0</v>
+      </c>
+      <c r="AE16" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF16">
+        <v>0</v>
+      </c>
+      <c r="AG16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1586280409</v>
+      </c>
+      <c r="B17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17">
+        <v>25443020</v>
+      </c>
+      <c r="E17" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17" s="1">
+        <v>43928</v>
+      </c>
+      <c r="G17" s="2">
+        <v>0.51862268518518517</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="J17" t="s">
+        <v>33</v>
+      </c>
+      <c r="K17">
+        <v>0.16159999999999999</v>
+      </c>
+      <c r="L17">
+        <v>0.16919999999999999</v>
+      </c>
+      <c r="M17">
+        <v>0.504</v>
+      </c>
+      <c r="N17">
+        <v>0.11559999999999999</v>
+      </c>
+      <c r="O17">
+        <v>1570</v>
+      </c>
+      <c r="P17">
+        <v>6.1400000000000003E-2</v>
+      </c>
+      <c r="Q17">
+        <v>1.9260999999999999</v>
+      </c>
+      <c r="R17">
+        <v>-4.0000000000000002E-4</v>
+      </c>
+      <c r="S17">
+        <v>0.16120000000000001</v>
+      </c>
+      <c r="T17">
+        <v>0</v>
+      </c>
+      <c r="U17">
+        <v>0.16919999999999999</v>
+      </c>
+      <c r="V17">
+        <v>0</v>
+      </c>
+      <c r="W17">
+        <v>0.504</v>
+      </c>
+      <c r="X17">
+        <v>0</v>
+      </c>
+      <c r="Y17">
+        <v>0.11559999999999999</v>
+      </c>
+      <c r="Z17">
+        <v>0</v>
+      </c>
+      <c r="AA17" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB17">
+        <v>0</v>
+      </c>
+      <c r="AC17" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD17">
+        <v>0</v>
+      </c>
+      <c r="AE17" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF17">
+        <v>0</v>
+      </c>
+      <c r="AG17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1586279919</v>
+      </c>
+      <c r="B18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18">
+        <v>25443020</v>
+      </c>
+      <c r="E18" t="s">
+        <v>32</v>
+      </c>
+      <c r="F18" s="1">
+        <v>43928</v>
+      </c>
+      <c r="G18" s="2">
+        <v>0.51295138888888892</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="J18" t="s">
+        <v>33</v>
+      </c>
+      <c r="K18">
+        <v>0.16439999999999999</v>
+      </c>
+      <c r="L18">
+        <v>0.1656</v>
+      </c>
+      <c r="M18">
+        <v>0.50719999999999998</v>
+      </c>
+      <c r="N18">
+        <v>0.1168</v>
+      </c>
+      <c r="O18">
+        <v>1570</v>
+      </c>
+      <c r="P18">
+        <v>5.6500000000000002E-2</v>
+      </c>
+      <c r="Q18">
+        <v>1.9268000000000001</v>
+      </c>
+      <c r="R18">
+        <v>-4.0000000000000002E-4</v>
+      </c>
+      <c r="S18">
+        <v>0.16400000000000001</v>
+      </c>
+      <c r="T18">
+        <v>-4.0000000000000002E-4</v>
+      </c>
+      <c r="U18">
+        <v>0.16520000000000001</v>
+      </c>
+      <c r="V18">
+        <v>0</v>
+      </c>
+      <c r="W18">
+        <v>0.50719999999999998</v>
+      </c>
+      <c r="X18">
+        <v>0</v>
+      </c>
+      <c r="Y18">
+        <v>0.1168</v>
+      </c>
+      <c r="Z18">
+        <v>0</v>
+      </c>
+      <c r="AA18" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB18">
+        <v>0</v>
+      </c>
+      <c r="AC18" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD18">
+        <v>0</v>
+      </c>
+      <c r="AE18" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF18">
+        <v>0</v>
+      </c>
+      <c r="AG18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1586279874</v>
+      </c>
+      <c r="B19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19">
+        <v>25443020</v>
+      </c>
+      <c r="E19" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" s="1">
+        <v>43928</v>
+      </c>
+      <c r="G19" s="2">
+        <v>0.51243055555555561</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19">
+        <v>1</v>
+      </c>
+      <c r="J19" t="s">
+        <v>33</v>
+      </c>
+      <c r="K19">
+        <v>0.16159999999999999</v>
+      </c>
+      <c r="L19">
+        <v>0.16639999999999999</v>
+      </c>
+      <c r="M19">
+        <v>0.51</v>
+      </c>
+      <c r="N19">
+        <v>0.1196</v>
+      </c>
+      <c r="O19">
+        <v>1570</v>
+      </c>
+      <c r="P19">
+        <v>5.9200000000000003E-2</v>
+      </c>
+      <c r="Q19">
+        <v>1.9169</v>
+      </c>
+      <c r="R19">
+        <v>-4.0000000000000002E-4</v>
+      </c>
+      <c r="S19">
+        <v>0.16120000000000001</v>
+      </c>
+      <c r="T19">
+        <v>-4.0000000000000002E-4</v>
+      </c>
+      <c r="U19">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="V19">
+        <v>0</v>
+      </c>
+      <c r="W19">
+        <v>0.51</v>
+      </c>
+      <c r="X19">
+        <v>0</v>
+      </c>
+      <c r="Y19">
+        <v>0.1196</v>
+      </c>
+      <c r="Z19">
+        <v>0</v>
+      </c>
+      <c r="AA19" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB19">
+        <v>0</v>
+      </c>
+      <c r="AC19" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD19">
+        <v>0</v>
+      </c>
+      <c r="AE19" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF19">
+        <v>0</v>
+      </c>
+      <c r="AG19" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1586279193</v>
+      </c>
+      <c r="B20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20">
+        <v>25443020</v>
+      </c>
+      <c r="E20" t="s">
+        <v>32</v>
+      </c>
+      <c r="F20" s="1">
+        <v>43928</v>
+      </c>
+      <c r="G20" s="2">
+        <v>0.50453703703703701</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
+      <c r="J20" t="s">
+        <v>33</v>
+      </c>
+      <c r="K20">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="L20">
+        <v>0.1636</v>
+      </c>
+      <c r="M20">
+        <v>0.51200000000000001</v>
+      </c>
+      <c r="N20">
+        <v>0.12039999999999999</v>
+      </c>
+      <c r="O20">
+        <v>1570</v>
+      </c>
+      <c r="P20">
+        <v>6.4299999999999996E-2</v>
+      </c>
+      <c r="Q20">
+        <v>1.9185000000000001</v>
+      </c>
+      <c r="R20">
+        <v>0</v>
+      </c>
+      <c r="S20">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="T20">
+        <v>0</v>
+      </c>
+      <c r="U20">
+        <v>0.1636</v>
+      </c>
+      <c r="V20">
+        <v>-4.0000000000000002E-4</v>
+      </c>
+      <c r="W20">
+        <v>0.51160000000000005</v>
+      </c>
+      <c r="X20">
+        <v>0</v>
+      </c>
+      <c r="Y20">
+        <v>0.12039999999999999</v>
+      </c>
+      <c r="Z20">
+        <v>0</v>
+      </c>
+      <c r="AA20" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB20">
+        <v>0</v>
+      </c>
+      <c r="AC20" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD20">
+        <v>0</v>
+      </c>
+      <c r="AE20" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF20">
+        <v>0</v>
+      </c>
+      <c r="AG20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1586279099</v>
+      </c>
+      <c r="B21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21">
+        <v>25443020</v>
+      </c>
+      <c r="E21" t="s">
+        <v>32</v>
+      </c>
+      <c r="F21" s="1">
+        <v>43928</v>
+      </c>
+      <c r="G21" s="2">
+        <v>0.50346064814814817</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21">
+        <v>1</v>
+      </c>
+      <c r="J21" t="s">
+        <v>33</v>
+      </c>
+      <c r="K21">
+        <v>0.1628</v>
+      </c>
+      <c r="L21">
+        <v>0.1668</v>
+      </c>
+      <c r="M21">
+        <v>0.51119999999999999</v>
+      </c>
+      <c r="N21">
+        <v>0.1212</v>
+      </c>
+      <c r="O21">
+        <v>1570</v>
+      </c>
+      <c r="P21">
+        <v>5.7500000000000002E-2</v>
+      </c>
+      <c r="Q21">
+        <v>1.9297</v>
+      </c>
+      <c r="R21">
+        <v>0</v>
+      </c>
+      <c r="S21">
+        <v>0.1628</v>
+      </c>
+      <c r="T21">
+        <v>0</v>
+      </c>
+      <c r="U21">
+        <v>0.1668</v>
+      </c>
+      <c r="V21">
+        <v>0</v>
+      </c>
+      <c r="W21">
+        <v>0.51119999999999999</v>
+      </c>
+      <c r="X21">
+        <v>0</v>
+      </c>
+      <c r="Y21">
+        <v>0.1212</v>
+      </c>
+      <c r="Z21">
+        <v>0</v>
+      </c>
+      <c r="AA21" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB21">
+        <v>0</v>
+      </c>
+      <c r="AC21" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD21">
+        <v>0</v>
+      </c>
+      <c r="AE21" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF21">
+        <v>0</v>
+      </c>
+      <c r="AG21" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>1586278479</v>
+      </c>
+      <c r="B22" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22">
+        <v>25443020</v>
+      </c>
+      <c r="E22" t="s">
+        <v>32</v>
+      </c>
+      <c r="F22" s="1">
+        <v>43928</v>
+      </c>
+      <c r="G22" s="2">
+        <v>0.49626157407407406</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <v>1</v>
+      </c>
+      <c r="J22" t="s">
+        <v>33</v>
+      </c>
+      <c r="K22">
+        <v>0.17</v>
+      </c>
+      <c r="L22">
+        <v>0.15720000000000001</v>
+      </c>
+      <c r="M22">
+        <v>0.49959999999999999</v>
+      </c>
+      <c r="N22">
+        <v>0.1192</v>
+      </c>
+      <c r="O22">
+        <v>1570</v>
+      </c>
+      <c r="P22">
+        <v>6.7100000000000007E-2</v>
+      </c>
+      <c r="Q22">
+        <v>1.9280999999999999</v>
+      </c>
+      <c r="R22">
+        <v>0</v>
+      </c>
+      <c r="S22">
+        <v>0.17</v>
+      </c>
+      <c r="T22">
+        <v>-4.0000000000000002E-4</v>
+      </c>
+      <c r="U22">
+        <v>0.15679999999999999</v>
+      </c>
+      <c r="V22">
+        <v>0</v>
+      </c>
+      <c r="W22">
+        <v>0.49959999999999999</v>
+      </c>
+      <c r="X22">
+        <v>-4.0000000000000002E-4</v>
+      </c>
+      <c r="Y22">
+        <v>0.1188</v>
+      </c>
+      <c r="Z22">
+        <v>0</v>
+      </c>
+      <c r="AA22" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB22">
+        <v>0</v>
+      </c>
+      <c r="AC22" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD22">
+        <v>0</v>
+      </c>
+      <c r="AE22" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF22">
+        <v>0</v>
+      </c>
+      <c r="AG22" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>1586278430</v>
+      </c>
+      <c r="B23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" t="s">
+        <v>31</v>
+      </c>
+      <c r="D23">
+        <v>25443020</v>
+      </c>
+      <c r="E23" t="s">
+        <v>32</v>
+      </c>
+      <c r="F23" s="1">
+        <v>43928</v>
+      </c>
+      <c r="G23" s="2">
+        <v>0.49571759259259257</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23">
+        <v>1</v>
+      </c>
+      <c r="J23" t="s">
+        <v>33</v>
+      </c>
+      <c r="K23">
+        <v>0.16400000000000001</v>
+      </c>
+      <c r="L23">
+        <v>0.15759999999999999</v>
+      </c>
+      <c r="M23">
+        <v>0.50960000000000005</v>
+      </c>
+      <c r="N23">
+        <v>0.1208</v>
+      </c>
+      <c r="O23">
+        <v>1570</v>
+      </c>
+      <c r="P23">
+        <v>5.8700000000000002E-2</v>
+      </c>
+      <c r="Q23">
+        <v>1.9188000000000001</v>
+      </c>
+      <c r="R23">
+        <v>-4.0000000000000002E-4</v>
+      </c>
+      <c r="S23">
+        <v>0.1636</v>
+      </c>
+      <c r="T23">
         <v>-8.0000000000000004E-4</v>
       </c>
-      <c r="S11">
+      <c r="U23">
+        <v>0.15679999999999999</v>
+      </c>
+      <c r="V23">
+        <v>0</v>
+      </c>
+      <c r="W23">
+        <v>0.50960000000000005</v>
+      </c>
+      <c r="X23">
+        <v>0</v>
+      </c>
+      <c r="Y23">
+        <v>0.1208</v>
+      </c>
+      <c r="Z23">
+        <v>0</v>
+      </c>
+      <c r="AA23" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB23">
+        <v>0</v>
+      </c>
+      <c r="AC23" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD23">
+        <v>0</v>
+      </c>
+      <c r="AE23" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF23">
+        <v>0</v>
+      </c>
+      <c r="AG23" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>1586277993</v>
+      </c>
+      <c r="B24" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24">
+        <v>25443020</v>
+      </c>
+      <c r="E24" t="s">
+        <v>32</v>
+      </c>
+      <c r="F24" s="1">
+        <v>43928</v>
+      </c>
+      <c r="G24" s="2">
+        <v>0.49065972222222221</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+      <c r="I24">
+        <v>1</v>
+      </c>
+      <c r="J24" t="s">
+        <v>33</v>
+      </c>
+      <c r="K24">
+        <v>0.16</v>
+      </c>
+      <c r="L24">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="M24">
+        <v>0.51160000000000005</v>
+      </c>
+      <c r="N24">
+        <v>0.1192</v>
+      </c>
+      <c r="O24">
+        <v>1570</v>
+      </c>
+      <c r="P24">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="Q24">
+        <v>1.9174</v>
+      </c>
+      <c r="R24">
+        <v>0</v>
+      </c>
+      <c r="S24">
+        <v>0.16</v>
+      </c>
+      <c r="T24">
+        <v>0</v>
+      </c>
+      <c r="U24">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="V24">
+        <v>0</v>
+      </c>
+      <c r="W24">
+        <v>0.51160000000000005</v>
+      </c>
+      <c r="X24">
+        <v>0</v>
+      </c>
+      <c r="Y24">
+        <v>0.1192</v>
+      </c>
+      <c r="Z24">
+        <v>0</v>
+      </c>
+      <c r="AA24" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB24">
+        <v>0</v>
+      </c>
+      <c r="AC24" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD24">
+        <v>0</v>
+      </c>
+      <c r="AE24" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF24">
+        <v>0</v>
+      </c>
+      <c r="AG24" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>1586277943</v>
+      </c>
+      <c r="B25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" t="s">
+        <v>31</v>
+      </c>
+      <c r="D25">
+        <v>25443020</v>
+      </c>
+      <c r="E25" t="s">
+        <v>32</v>
+      </c>
+      <c r="F25" s="1">
+        <v>43928</v>
+      </c>
+      <c r="G25" s="2">
+        <v>0.49006944444444445</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+      <c r="I25">
+        <v>1</v>
+      </c>
+      <c r="J25" t="s">
+        <v>33</v>
+      </c>
+      <c r="K25">
+        <v>0.16039999999999999</v>
+      </c>
+      <c r="L25">
+        <v>0.1648</v>
+      </c>
+      <c r="M25">
+        <v>0.51039999999999996</v>
+      </c>
+      <c r="N25">
+        <v>0.12039999999999999</v>
+      </c>
+      <c r="O25">
+        <v>1570</v>
+      </c>
+      <c r="P25">
+        <v>6.4299999999999996E-2</v>
+      </c>
+      <c r="Q25">
+        <v>1.9312</v>
+      </c>
+      <c r="R25">
+        <v>-4.0000000000000002E-4</v>
+      </c>
+      <c r="S25">
+        <v>0.16</v>
+      </c>
+      <c r="T25">
+        <v>0</v>
+      </c>
+      <c r="U25">
+        <v>0.1648</v>
+      </c>
+      <c r="V25">
+        <v>0</v>
+      </c>
+      <c r="W25">
+        <v>0.51039999999999996</v>
+      </c>
+      <c r="X25">
+        <v>0</v>
+      </c>
+      <c r="Y25">
+        <v>0.12039999999999999</v>
+      </c>
+      <c r="Z25">
+        <v>0</v>
+      </c>
+      <c r="AA25" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB25">
+        <v>0</v>
+      </c>
+      <c r="AC25" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD25">
+        <v>0</v>
+      </c>
+      <c r="AE25" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF25">
+        <v>0</v>
+      </c>
+      <c r="AG25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>1586277380</v>
+      </c>
+      <c r="B26" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26">
+        <v>25443020</v>
+      </c>
+      <c r="E26" t="s">
+        <v>32</v>
+      </c>
+      <c r="F26" s="1">
+        <v>43928</v>
+      </c>
+      <c r="G26" s="2">
+        <v>0.48356481481481484</v>
+      </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+      <c r="I26">
+        <v>1</v>
+      </c>
+      <c r="J26" t="s">
+        <v>33</v>
+      </c>
+      <c r="K26">
+        <v>0.16239999999999999</v>
+      </c>
+      <c r="L26">
+        <v>0.15840000000000001</v>
+      </c>
+      <c r="M26">
+        <v>0.50600000000000001</v>
+      </c>
+      <c r="N26">
+        <v>0.11600000000000001</v>
+      </c>
+      <c r="O26">
+        <v>1570</v>
+      </c>
+      <c r="P26">
+        <v>5.3900000000000003E-2</v>
+      </c>
+      <c r="Q26">
+        <v>1.9134</v>
+      </c>
+      <c r="R26">
+        <v>0</v>
+      </c>
+      <c r="S26">
+        <v>0.16239999999999999</v>
+      </c>
+      <c r="T26">
+        <v>0</v>
+      </c>
+      <c r="U26">
+        <v>0.15840000000000001</v>
+      </c>
+      <c r="V26">
+        <v>-1.1999999999999999E-3</v>
+      </c>
+      <c r="W26">
+        <v>0.50480000000000003</v>
+      </c>
+      <c r="X26">
+        <v>-4.0000000000000002E-4</v>
+      </c>
+      <c r="Y26">
+        <v>0.11559999999999999</v>
+      </c>
+      <c r="Z26">
+        <v>0</v>
+      </c>
+      <c r="AA26" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB26">
+        <v>0</v>
+      </c>
+      <c r="AC26" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD26">
+        <v>0</v>
+      </c>
+      <c r="AE26" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF26">
+        <v>0</v>
+      </c>
+      <c r="AG26" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1586277321</v>
+      </c>
+      <c r="B27" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" t="s">
+        <v>31</v>
+      </c>
+      <c r="D27">
+        <v>25443020</v>
+      </c>
+      <c r="E27" t="s">
+        <v>32</v>
+      </c>
+      <c r="F27" s="1">
+        <v>43928</v>
+      </c>
+      <c r="G27" s="2">
+        <v>0.48283564814814817</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <v>1</v>
+      </c>
+      <c r="J27" t="s">
+        <v>33</v>
+      </c>
+      <c r="K27">
+        <v>0.15959999999999999</v>
+      </c>
+      <c r="L27">
+        <v>0.1608</v>
+      </c>
+      <c r="M27">
+        <v>0.51519999999999999</v>
+      </c>
+      <c r="N27">
+        <v>0.1172</v>
+      </c>
+      <c r="O27">
+        <v>1570</v>
+      </c>
+      <c r="P27">
+        <v>6.7599999999999993E-2</v>
+      </c>
+      <c r="Q27">
+        <v>1.9202999999999999</v>
+      </c>
+      <c r="R27">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="S27">
+        <v>0.16</v>
+      </c>
+      <c r="T27">
+        <v>-8.0000000000000004E-4</v>
+      </c>
+      <c r="U27">
+        <v>0.16</v>
+      </c>
+      <c r="V27">
+        <v>-8.0000000000000004E-4</v>
+      </c>
+      <c r="W27">
+        <v>0.51439999999999997</v>
+      </c>
+      <c r="X27">
+        <v>0</v>
+      </c>
+      <c r="Y27">
+        <v>0.1172</v>
+      </c>
+      <c r="Z27">
+        <v>0</v>
+      </c>
+      <c r="AA27" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB27">
+        <v>0</v>
+      </c>
+      <c r="AC27" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD27">
+        <v>0</v>
+      </c>
+      <c r="AE27" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF27">
+        <v>0</v>
+      </c>
+      <c r="AG27" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>1586276784</v>
+      </c>
+      <c r="B28" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" t="s">
+        <v>31</v>
+      </c>
+      <c r="D28">
+        <v>25443020</v>
+      </c>
+      <c r="E28" t="s">
+        <v>32</v>
+      </c>
+      <c r="F28" s="1">
+        <v>43928</v>
+      </c>
+      <c r="G28" s="2">
+        <v>0.47666666666666663</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="I28">
+        <v>1</v>
+      </c>
+      <c r="J28" t="s">
+        <v>33</v>
+      </c>
+      <c r="K28">
+        <v>0.16880000000000001</v>
+      </c>
+      <c r="L28">
+        <v>0.15959999999999999</v>
+      </c>
+      <c r="M28">
+        <v>0.50160000000000005</v>
+      </c>
+      <c r="N28">
+        <v>0.12039999999999999</v>
+      </c>
+      <c r="O28">
+        <v>1570</v>
+      </c>
+      <c r="P28">
+        <v>5.7200000000000001E-2</v>
+      </c>
+      <c r="Q28">
+        <v>1.9216</v>
+      </c>
+      <c r="R28">
+        <v>-4.0000000000000002E-4</v>
+      </c>
+      <c r="S28">
+        <v>0.16839999999999999</v>
+      </c>
+      <c r="T28">
+        <v>-8.0000000000000004E-4</v>
+      </c>
+      <c r="U28">
+        <v>0.1588</v>
+      </c>
+      <c r="V28">
+        <v>0</v>
+      </c>
+      <c r="W28">
+        <v>0.50160000000000005</v>
+      </c>
+      <c r="X28">
+        <v>0</v>
+      </c>
+      <c r="Y28">
+        <v>0.12039999999999999</v>
+      </c>
+      <c r="Z28">
+        <v>0</v>
+      </c>
+      <c r="AA28" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB28">
+        <v>0</v>
+      </c>
+      <c r="AC28" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD28">
+        <v>0</v>
+      </c>
+      <c r="AE28" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF28">
+        <v>0</v>
+      </c>
+      <c r="AG28" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>1586276695</v>
+      </c>
+      <c r="B29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" t="s">
+        <v>31</v>
+      </c>
+      <c r="D29">
+        <v>25443020</v>
+      </c>
+      <c r="E29" t="s">
+        <v>32</v>
+      </c>
+      <c r="F29" s="1">
+        <v>43928</v>
+      </c>
+      <c r="G29" s="2">
+        <v>0.47562499999999996</v>
+      </c>
+      <c r="H29">
+        <v>1</v>
+      </c>
+      <c r="I29">
+        <v>1</v>
+      </c>
+      <c r="J29" t="s">
+        <v>33</v>
+      </c>
+      <c r="K29">
+        <v>0.1736</v>
+      </c>
+      <c r="L29">
+        <v>0.16</v>
+      </c>
+      <c r="M29">
+        <v>0.50160000000000005</v>
+      </c>
+      <c r="N29">
+        <v>0.1188</v>
+      </c>
+      <c r="O29">
+        <v>1570</v>
+      </c>
+      <c r="P29">
+        <v>6.0600000000000001E-2</v>
+      </c>
+      <c r="Q29">
+        <v>1.9176</v>
+      </c>
+      <c r="R29">
+        <v>-8.0000000000000004E-4</v>
+      </c>
+      <c r="S29">
+        <v>0.17280000000000001</v>
+      </c>
+      <c r="T29">
+        <v>0</v>
+      </c>
+      <c r="U29">
+        <v>0.16</v>
+      </c>
+      <c r="V29">
+        <v>0</v>
+      </c>
+      <c r="W29">
+        <v>0.50160000000000005</v>
+      </c>
+      <c r="X29">
+        <v>0</v>
+      </c>
+      <c r="Y29">
+        <v>0.1188</v>
+      </c>
+      <c r="Z29">
+        <v>0</v>
+      </c>
+      <c r="AA29" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB29">
+        <v>0</v>
+      </c>
+      <c r="AC29" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD29">
+        <v>0</v>
+      </c>
+      <c r="AE29" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF29">
+        <v>0</v>
+      </c>
+      <c r="AG29" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>1586276108</v>
+      </c>
+      <c r="B30" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" t="s">
+        <v>31</v>
+      </c>
+      <c r="D30">
+        <v>25443020</v>
+      </c>
+      <c r="E30" t="s">
+        <v>32</v>
+      </c>
+      <c r="F30" s="1">
+        <v>43928</v>
+      </c>
+      <c r="G30" s="2">
+        <v>0.46883101851851849</v>
+      </c>
+      <c r="H30">
+        <v>1</v>
+      </c>
+      <c r="I30">
+        <v>1</v>
+      </c>
+      <c r="J30" t="s">
+        <v>33</v>
+      </c>
+      <c r="K30">
+        <v>0.1772</v>
+      </c>
+      <c r="L30">
+        <v>0.1636</v>
+      </c>
+      <c r="M30">
+        <v>0.5</v>
+      </c>
+      <c r="N30">
+        <v>0.12280000000000001</v>
+      </c>
+      <c r="O30">
+        <v>1570</v>
+      </c>
+      <c r="P30">
+        <v>7.0699999999999999E-2</v>
+      </c>
+      <c r="Q30">
+        <v>1.9257</v>
+      </c>
+      <c r="R30">
+        <v>-1.1999999999999999E-3</v>
+      </c>
+      <c r="S30">
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="T30">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="U30">
+        <v>0.16400000000000001</v>
+      </c>
+      <c r="V30">
+        <v>0</v>
+      </c>
+      <c r="W30">
+        <v>0.5</v>
+      </c>
+      <c r="X30">
+        <v>0</v>
+      </c>
+      <c r="Y30">
+        <v>0.12280000000000001</v>
+      </c>
+      <c r="Z30">
+        <v>0</v>
+      </c>
+      <c r="AA30" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB30">
+        <v>0</v>
+      </c>
+      <c r="AC30" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD30">
+        <v>0</v>
+      </c>
+      <c r="AE30" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF30">
+        <v>0</v>
+      </c>
+      <c r="AG30" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>1586276057</v>
+      </c>
+      <c r="B31" t="s">
+        <v>30</v>
+      </c>
+      <c r="C31" t="s">
+        <v>31</v>
+      </c>
+      <c r="D31">
+        <v>25443020</v>
+      </c>
+      <c r="E31" t="s">
+        <v>32</v>
+      </c>
+      <c r="F31" s="1">
+        <v>43928</v>
+      </c>
+      <c r="G31" s="2">
+        <v>0.46825231481481483</v>
+      </c>
+      <c r="H31">
+        <v>1</v>
+      </c>
+      <c r="I31">
+        <v>1</v>
+      </c>
+      <c r="J31" t="s">
+        <v>33</v>
+      </c>
+      <c r="K31">
+        <v>0.1772</v>
+      </c>
+      <c r="L31">
+        <v>0.16520000000000001</v>
+      </c>
+      <c r="M31">
+        <v>0.50519999999999998</v>
+      </c>
+      <c r="N31">
+        <v>0.1232</v>
+      </c>
+      <c r="O31">
+        <v>1570</v>
+      </c>
+      <c r="P31">
+        <v>6.2700000000000006E-2</v>
+      </c>
+      <c r="Q31">
+        <v>1.9266000000000001</v>
+      </c>
+      <c r="R31">
+        <v>0</v>
+      </c>
+      <c r="S31">
+        <v>0.1772</v>
+      </c>
+      <c r="T31">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="U31">
+        <v>0.1656</v>
+      </c>
+      <c r="V31">
+        <v>0</v>
+      </c>
+      <c r="W31">
+        <v>0.50519999999999998</v>
+      </c>
+      <c r="X31">
+        <v>0</v>
+      </c>
+      <c r="Y31">
+        <v>0.1232</v>
+      </c>
+      <c r="Z31">
+        <v>0</v>
+      </c>
+      <c r="AA31" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB31">
+        <v>0</v>
+      </c>
+      <c r="AC31" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD31">
+        <v>0</v>
+      </c>
+      <c r="AE31" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF31">
+        <v>0</v>
+      </c>
+      <c r="AG31" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>1586275476</v>
+      </c>
+      <c r="B32" t="s">
+        <v>30</v>
+      </c>
+      <c r="C32" t="s">
+        <v>31</v>
+      </c>
+      <c r="D32">
+        <v>25443020</v>
+      </c>
+      <c r="E32" t="s">
+        <v>32</v>
+      </c>
+      <c r="F32" s="1">
+        <v>43928</v>
+      </c>
+      <c r="G32" s="2">
+        <v>0.46152777777777776</v>
+      </c>
+      <c r="H32">
+        <v>1</v>
+      </c>
+      <c r="I32">
+        <v>1</v>
+      </c>
+      <c r="J32" t="s">
+        <v>33</v>
+      </c>
+      <c r="K32">
+        <v>0.1628</v>
+      </c>
+      <c r="L32">
+        <v>0.16159999999999999</v>
+      </c>
+      <c r="M32">
+        <v>0.51639999999999997</v>
+      </c>
+      <c r="N32">
+        <v>0.12</v>
+      </c>
+      <c r="O32">
+        <v>1570</v>
+      </c>
+      <c r="P32">
+        <v>6.4799999999999996E-2</v>
+      </c>
+      <c r="Q32">
+        <v>1.9253</v>
+      </c>
+      <c r="R32">
+        <v>-4.0000000000000002E-4</v>
+      </c>
+      <c r="S32">
+        <v>0.16239999999999999</v>
+      </c>
+      <c r="T32">
+        <v>0</v>
+      </c>
+      <c r="U32">
+        <v>0.16159999999999999</v>
+      </c>
+      <c r="V32">
+        <v>0</v>
+      </c>
+      <c r="W32">
+        <v>0.51639999999999997</v>
+      </c>
+      <c r="X32">
+        <v>0</v>
+      </c>
+      <c r="Y32">
+        <v>0.12</v>
+      </c>
+      <c r="Z32">
+        <v>0</v>
+      </c>
+      <c r="AA32" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB32">
+        <v>0</v>
+      </c>
+      <c r="AC32" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD32">
+        <v>0</v>
+      </c>
+      <c r="AE32" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF32">
+        <v>0</v>
+      </c>
+      <c r="AG32" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>1586275363</v>
+      </c>
+      <c r="B33" t="s">
+        <v>30</v>
+      </c>
+      <c r="C33" t="s">
+        <v>31</v>
+      </c>
+      <c r="D33">
+        <v>25443020</v>
+      </c>
+      <c r="E33" t="s">
+        <v>32</v>
+      </c>
+      <c r="F33" s="1">
+        <v>43928</v>
+      </c>
+      <c r="G33" s="2">
+        <v>0.46021990740740742</v>
+      </c>
+      <c r="H33">
+        <v>1</v>
+      </c>
+      <c r="I33">
+        <v>1</v>
+      </c>
+      <c r="J33" t="s">
+        <v>33</v>
+      </c>
+      <c r="K33">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="L33">
+        <v>0.16</v>
+      </c>
+      <c r="M33">
+        <v>0.51119999999999999</v>
+      </c>
+      <c r="N33">
+        <v>0.1208</v>
+      </c>
+      <c r="O33">
+        <v>1570</v>
+      </c>
+      <c r="P33">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="Q33">
+        <v>1.9209000000000001</v>
+      </c>
+      <c r="R33">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="S33">
+        <v>0.16239999999999999</v>
+      </c>
+      <c r="T33">
+        <v>-4.0000000000000002E-4</v>
+      </c>
+      <c r="U33">
+        <v>0.15959999999999999</v>
+      </c>
+      <c r="V33">
+        <v>0</v>
+      </c>
+      <c r="W33">
+        <v>0.51119999999999999</v>
+      </c>
+      <c r="X33">
+        <v>-4.0000000000000002E-4</v>
+      </c>
+      <c r="Y33">
+        <v>0.12039999999999999</v>
+      </c>
+      <c r="Z33">
+        <v>0</v>
+      </c>
+      <c r="AA33" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB33">
+        <v>0</v>
+      </c>
+      <c r="AC33" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD33">
+        <v>0</v>
+      </c>
+      <c r="AE33" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF33">
+        <v>0</v>
+      </c>
+      <c r="AG33" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="34" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>1586273102</v>
+      </c>
+      <c r="B34" t="s">
+        <v>30</v>
+      </c>
+      <c r="C34" t="s">
+        <v>31</v>
+      </c>
+      <c r="D34">
+        <v>25443020</v>
+      </c>
+      <c r="E34" t="s">
+        <v>32</v>
+      </c>
+      <c r="F34" s="1">
+        <v>43928</v>
+      </c>
+      <c r="G34" s="2">
+        <v>0.43405092592592592</v>
+      </c>
+      <c r="H34">
+        <v>1</v>
+      </c>
+      <c r="I34">
+        <v>1</v>
+      </c>
+      <c r="J34" t="s">
+        <v>33</v>
+      </c>
+      <c r="K34">
+        <v>0.16159999999999999</v>
+      </c>
+      <c r="L34">
+        <v>0.16400000000000001</v>
+      </c>
+      <c r="M34">
+        <v>0.51919999999999999</v>
+      </c>
+      <c r="N34">
+        <v>0.1208</v>
+      </c>
+      <c r="O34">
+        <v>1570</v>
+      </c>
+      <c r="P34">
+        <v>6.5500000000000003E-2</v>
+      </c>
+      <c r="Q34">
+        <v>1.9178999999999999</v>
+      </c>
+      <c r="R34">
+        <v>-4.0000000000000002E-4</v>
+      </c>
+      <c r="S34">
+        <v>0.16120000000000001</v>
+      </c>
+      <c r="T34">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="U34">
         <v>0.16439999999999999</v>
       </c>
-      <c r="T11">
-        <v>1.7756000000000001</v>
-      </c>
-      <c r="U11">
-        <v>1.9408000000000001</v>
-      </c>
-      <c r="V11">
+      <c r="V34">
+        <v>-4.0000000000000002E-4</v>
+      </c>
+      <c r="W34">
+        <v>0.51880000000000004</v>
+      </c>
+      <c r="X34">
+        <v>0</v>
+      </c>
+      <c r="Y34">
+        <v>0.1208</v>
+      </c>
+      <c r="Z34">
+        <v>0</v>
+      </c>
+      <c r="AA34" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB34">
+        <v>0</v>
+      </c>
+      <c r="AC34" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD34">
+        <v>0</v>
+      </c>
+      <c r="AE34" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF34">
+        <v>0</v>
+      </c>
+      <c r="AG34" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>1586273053</v>
+      </c>
+      <c r="B35" t="s">
+        <v>30</v>
+      </c>
+      <c r="C35" t="s">
+        <v>31</v>
+      </c>
+      <c r="D35">
+        <v>25443020</v>
+      </c>
+      <c r="E35" t="s">
+        <v>32</v>
+      </c>
+      <c r="F35" s="1">
+        <v>43928</v>
+      </c>
+      <c r="G35" s="2">
+        <v>0.4334837962962963</v>
+      </c>
+      <c r="H35">
+        <v>1</v>
+      </c>
+      <c r="I35">
+        <v>1</v>
+      </c>
+      <c r="J35" t="s">
+        <v>33</v>
+      </c>
+      <c r="K35">
+        <v>0.1588</v>
+      </c>
+      <c r="L35">
+        <v>0.1656</v>
+      </c>
+      <c r="M35">
+        <v>0.51680000000000004</v>
+      </c>
+      <c r="N35">
+        <v>0.1196</v>
+      </c>
+      <c r="O35">
+        <v>1570</v>
+      </c>
+      <c r="P35">
+        <v>5.9299999999999999E-2</v>
+      </c>
+      <c r="Q35">
+        <v>1.9080999999999999</v>
+      </c>
+      <c r="R35">
+        <v>0</v>
+      </c>
+      <c r="S35">
+        <v>0.1588</v>
+      </c>
+      <c r="T35">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="U35">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="V35">
+        <v>0</v>
+      </c>
+      <c r="W35">
+        <v>0.51680000000000004</v>
+      </c>
+      <c r="X35">
+        <v>0</v>
+      </c>
+      <c r="Y35">
+        <v>0.1196</v>
+      </c>
+      <c r="Z35">
+        <v>0</v>
+      </c>
+      <c r="AA35" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB35">
+        <v>0</v>
+      </c>
+      <c r="AC35" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD35">
+        <v>0</v>
+      </c>
+      <c r="AE35" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF35">
+        <v>0</v>
+      </c>
+      <c r="AG35" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>1586272528</v>
+      </c>
+      <c r="B36" t="s">
+        <v>30</v>
+      </c>
+      <c r="C36" t="s">
+        <v>31</v>
+      </c>
+      <c r="D36">
+        <v>25443020</v>
+      </c>
+      <c r="E36" t="s">
+        <v>32</v>
+      </c>
+      <c r="F36" s="1">
+        <v>43928</v>
+      </c>
+      <c r="G36" s="2">
+        <v>0.42739583333333336</v>
+      </c>
+      <c r="H36">
+        <v>1</v>
+      </c>
+      <c r="I36">
+        <v>1</v>
+      </c>
+      <c r="J36" t="s">
+        <v>33</v>
+      </c>
+      <c r="K36">
+        <v>0.16880000000000001</v>
+      </c>
+      <c r="L36">
+        <v>0.15720000000000001</v>
+      </c>
+      <c r="M36">
+        <v>0.50919999999999999</v>
+      </c>
+      <c r="N36">
+        <v>0.1208</v>
+      </c>
+      <c r="O36">
+        <v>1570</v>
+      </c>
+      <c r="P36">
+        <v>6.3200000000000006E-2</v>
+      </c>
+      <c r="Q36">
+        <v>1.9140999999999999</v>
+      </c>
+      <c r="R36">
+        <v>0</v>
+      </c>
+      <c r="S36">
+        <v>0.16880000000000001</v>
+      </c>
+      <c r="T36">
+        <v>0</v>
+      </c>
+      <c r="U36">
+        <v>0.15720000000000001</v>
+      </c>
+      <c r="V36">
+        <v>0</v>
+      </c>
+      <c r="W36">
+        <v>0.50919999999999999</v>
+      </c>
+      <c r="X36">
+        <v>0</v>
+      </c>
+      <c r="Y36">
+        <v>0.1208</v>
+      </c>
+      <c r="Z36">
+        <v>0</v>
+      </c>
+      <c r="AA36" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB36">
+        <v>0</v>
+      </c>
+      <c r="AC36" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD36">
+        <v>0</v>
+      </c>
+      <c r="AE36" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF36">
+        <v>0</v>
+      </c>
+      <c r="AG36" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>1586272479</v>
+      </c>
+      <c r="B37" t="s">
+        <v>30</v>
+      </c>
+      <c r="C37" t="s">
+        <v>31</v>
+      </c>
+      <c r="D37">
+        <v>25443020</v>
+      </c>
+      <c r="E37" t="s">
+        <v>32</v>
+      </c>
+      <c r="F37" s="1">
+        <v>43928</v>
+      </c>
+      <c r="G37" s="2">
+        <v>0.42682870370370374</v>
+      </c>
+      <c r="H37">
+        <v>1</v>
+      </c>
+      <c r="I37">
+        <v>1</v>
+      </c>
+      <c r="J37" t="s">
+        <v>33</v>
+      </c>
+      <c r="K37">
+        <v>0.17680000000000001</v>
+      </c>
+      <c r="L37">
+        <v>0.16</v>
+      </c>
+      <c r="M37">
+        <v>0.50680000000000003</v>
+      </c>
+      <c r="N37">
+        <v>0.12039999999999999</v>
+      </c>
+      <c r="O37">
+        <v>1570</v>
+      </c>
+      <c r="P37">
+        <v>5.2400000000000002E-2</v>
+      </c>
+      <c r="Q37">
+        <v>1.9081999999999999</v>
+      </c>
+      <c r="R37">
+        <v>-4.0000000000000002E-4</v>
+      </c>
+      <c r="S37">
+        <v>0.1764</v>
+      </c>
+      <c r="T37">
+        <v>-4.0000000000000002E-4</v>
+      </c>
+      <c r="U37">
+        <v>0.15959999999999999</v>
+      </c>
+      <c r="V37">
+        <v>0</v>
+      </c>
+      <c r="W37">
+        <v>0.50680000000000003</v>
+      </c>
+      <c r="X37">
+        <v>0</v>
+      </c>
+      <c r="Y37">
+        <v>0.12039999999999999</v>
+      </c>
+      <c r="Z37">
+        <v>0</v>
+      </c>
+      <c r="AA37" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB37">
+        <v>0</v>
+      </c>
+      <c r="AC37" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD37">
+        <v>0</v>
+      </c>
+      <c r="AE37" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF37">
+        <v>0</v>
+      </c>
+      <c r="AG37" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="38" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>1586271746</v>
+      </c>
+      <c r="B38" t="s">
+        <v>30</v>
+      </c>
+      <c r="C38" t="s">
+        <v>31</v>
+      </c>
+      <c r="D38">
+        <v>25443020</v>
+      </c>
+      <c r="E38" t="s">
+        <v>32</v>
+      </c>
+      <c r="F38" s="1">
+        <v>43928</v>
+      </c>
+      <c r="G38" s="2">
+        <v>0.41835648148148147</v>
+      </c>
+      <c r="H38">
+        <v>1</v>
+      </c>
+      <c r="I38">
+        <v>1</v>
+      </c>
+      <c r="J38" t="s">
+        <v>33</v>
+      </c>
+      <c r="K38">
         <v>0.1648</v>
       </c>
-      <c r="W11">
-        <v>0.66039999999999999</v>
-      </c>
-      <c r="X11">
-        <v>0.66120000000000001</v>
-      </c>
-      <c r="Y11">
-        <v>0.78320000000000001</v>
-      </c>
-      <c r="Z11">
-        <v>0</v>
-      </c>
-      <c r="AA11" t="s">
-        <v>34</v>
-      </c>
-      <c r="AB11">
-        <v>0</v>
-      </c>
-      <c r="AC11" t="s">
-        <v>34</v>
-      </c>
-      <c r="AD11">
-        <v>0</v>
-      </c>
-      <c r="AE11" t="s">
-        <v>34</v>
-      </c>
-      <c r="AF11">
-        <v>0</v>
-      </c>
-      <c r="AG11" t="s">
+      <c r="L38">
+        <v>0.17080000000000001</v>
+      </c>
+      <c r="M38">
+        <v>0.51439999999999997</v>
+      </c>
+      <c r="N38">
+        <v>0.1216</v>
+      </c>
+      <c r="O38">
+        <v>1570</v>
+      </c>
+      <c r="P38">
+        <v>5.67E-2</v>
+      </c>
+      <c r="Q38">
+        <v>1.9160999999999999</v>
+      </c>
+      <c r="R38">
+        <v>-1.1999999999999999E-3</v>
+      </c>
+      <c r="S38">
+        <v>0.1636</v>
+      </c>
+      <c r="T38">
+        <v>0</v>
+      </c>
+      <c r="U38">
+        <v>0.17080000000000001</v>
+      </c>
+      <c r="V38">
+        <v>0</v>
+      </c>
+      <c r="W38">
+        <v>0.51439999999999997</v>
+      </c>
+      <c r="X38">
+        <v>0</v>
+      </c>
+      <c r="Y38">
+        <v>0.1216</v>
+      </c>
+      <c r="Z38">
+        <v>0</v>
+      </c>
+      <c r="AA38" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB38">
+        <v>0</v>
+      </c>
+      <c r="AC38" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD38">
+        <v>0</v>
+      </c>
+      <c r="AE38" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF38">
+        <v>0</v>
+      </c>
+      <c r="AG38" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="39" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>1586271579</v>
+      </c>
+      <c r="B39" t="s">
+        <v>30</v>
+      </c>
+      <c r="C39" t="s">
+        <v>31</v>
+      </c>
+      <c r="D39">
+        <v>25443020</v>
+      </c>
+      <c r="E39" t="s">
+        <v>32</v>
+      </c>
+      <c r="F39" s="1">
+        <v>43928</v>
+      </c>
+      <c r="G39" s="2">
+        <v>0.41641203703703705</v>
+      </c>
+      <c r="H39">
+        <v>1</v>
+      </c>
+      <c r="I39">
+        <v>1</v>
+      </c>
+      <c r="J39" t="s">
+        <v>33</v>
+      </c>
+      <c r="K39">
+        <v>0.16520000000000001</v>
+      </c>
+      <c r="L39">
+        <v>0.16520000000000001</v>
+      </c>
+      <c r="M39">
+        <v>0.51080000000000003</v>
+      </c>
+      <c r="N39">
+        <v>0.12039999999999999</v>
+      </c>
+      <c r="O39">
+        <v>1570</v>
+      </c>
+      <c r="P39">
+        <v>5.8700000000000002E-2</v>
+      </c>
+      <c r="Q39">
+        <v>1.9196</v>
+      </c>
+      <c r="R39">
+        <v>-4.0000000000000002E-4</v>
+      </c>
+      <c r="S39">
+        <v>0.1648</v>
+      </c>
+      <c r="T39">
+        <v>0</v>
+      </c>
+      <c r="U39">
+        <v>0.16520000000000001</v>
+      </c>
+      <c r="V39">
+        <v>0</v>
+      </c>
+      <c r="W39">
+        <v>0.51080000000000003</v>
+      </c>
+      <c r="X39">
+        <v>0</v>
+      </c>
+      <c r="Y39">
+        <v>0.12039999999999999</v>
+      </c>
+      <c r="Z39">
+        <v>0</v>
+      </c>
+      <c r="AA39" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB39">
+        <v>0</v>
+      </c>
+      <c r="AC39" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD39">
+        <v>0</v>
+      </c>
+      <c r="AE39" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF39">
+        <v>0</v>
+      </c>
+      <c r="AG39" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="40" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>1586271033</v>
+      </c>
+      <c r="B40" t="s">
+        <v>30</v>
+      </c>
+      <c r="C40" t="s">
+        <v>31</v>
+      </c>
+      <c r="D40">
+        <v>25443020</v>
+      </c>
+      <c r="E40" t="s">
+        <v>32</v>
+      </c>
+      <c r="F40" s="1">
+        <v>43928</v>
+      </c>
+      <c r="G40" s="2">
+        <v>0.41009259259259262</v>
+      </c>
+      <c r="H40">
+        <v>1</v>
+      </c>
+      <c r="I40">
+        <v>1</v>
+      </c>
+      <c r="J40" t="s">
+        <v>33</v>
+      </c>
+      <c r="K40">
+        <v>0.1608</v>
+      </c>
+      <c r="L40">
+        <v>0.16239999999999999</v>
+      </c>
+      <c r="M40">
+        <v>0.51559999999999995</v>
+      </c>
+      <c r="N40">
+        <v>0.12</v>
+      </c>
+      <c r="O40">
+        <v>1570</v>
+      </c>
+      <c r="P40">
+        <v>5.4699999999999999E-2</v>
+      </c>
+      <c r="Q40">
+        <v>1.9174</v>
+      </c>
+      <c r="R40">
+        <v>-4.0000000000000002E-4</v>
+      </c>
+      <c r="S40">
+        <v>0.16039999999999999</v>
+      </c>
+      <c r="T40">
+        <v>0</v>
+      </c>
+      <c r="U40">
+        <v>0.16239999999999999</v>
+      </c>
+      <c r="V40">
+        <v>0</v>
+      </c>
+      <c r="W40">
+        <v>0.51559999999999995</v>
+      </c>
+      <c r="X40">
+        <v>-4.0000000000000002E-4</v>
+      </c>
+      <c r="Y40">
+        <v>0.1196</v>
+      </c>
+      <c r="Z40">
+        <v>0</v>
+      </c>
+      <c r="AA40" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB40">
+        <v>0</v>
+      </c>
+      <c r="AC40" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD40">
+        <v>0</v>
+      </c>
+      <c r="AE40" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF40">
+        <v>0</v>
+      </c>
+      <c r="AG40" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="41" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>1586270981</v>
+      </c>
+      <c r="B41" t="s">
+        <v>30</v>
+      </c>
+      <c r="C41" t="s">
+        <v>31</v>
+      </c>
+      <c r="D41">
+        <v>25443020</v>
+      </c>
+      <c r="E41" t="s">
+        <v>32</v>
+      </c>
+      <c r="F41" s="1">
+        <v>43928</v>
+      </c>
+      <c r="G41" s="2">
+        <v>0.40949074074074071</v>
+      </c>
+      <c r="H41">
+        <v>1</v>
+      </c>
+      <c r="I41">
+        <v>1</v>
+      </c>
+      <c r="J41" t="s">
+        <v>33</v>
+      </c>
+      <c r="K41">
+        <v>0.16320000000000001</v>
+      </c>
+      <c r="L41">
+        <v>0.16239999999999999</v>
+      </c>
+      <c r="M41">
+        <v>0.51839999999999997</v>
+      </c>
+      <c r="N41">
+        <v>0.1216</v>
+      </c>
+      <c r="O41">
+        <v>1570</v>
+      </c>
+      <c r="P41">
+        <v>5.6599999999999998E-2</v>
+      </c>
+      <c r="Q41">
+        <v>1.9065000000000001</v>
+      </c>
+      <c r="R41">
+        <v>0</v>
+      </c>
+      <c r="S41">
+        <v>0.16320000000000001</v>
+      </c>
+      <c r="T41">
+        <v>-1.1999999999999999E-3</v>
+      </c>
+      <c r="U41">
+        <v>0.16120000000000001</v>
+      </c>
+      <c r="V41">
+        <v>0</v>
+      </c>
+      <c r="W41">
+        <v>0.51839999999999997</v>
+      </c>
+      <c r="X41">
+        <v>0</v>
+      </c>
+      <c r="Y41">
+        <v>0.1216</v>
+      </c>
+      <c r="Z41">
+        <v>0</v>
+      </c>
+      <c r="AA41" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB41">
+        <v>0</v>
+      </c>
+      <c r="AC41" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD41">
+        <v>0</v>
+      </c>
+      <c r="AE41" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF41">
+        <v>0</v>
+      </c>
+      <c r="AG41" t="s">
         <v>34</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>